<commit_message>
Download path to github directory
Download path to github directory
</commit_message>
<xml_diff>
--- a/projects/sku-tracking/mister/raw-data/Mister-SKUs.xlsx
+++ b/projects/sku-tracking/mister/raw-data/Mister-SKUs.xlsx
@@ -1466,10 +1466,10 @@
         <v>50</v>
       </c>
       <c r="Q13" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R13" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S13" s="0" t="inlineStr">
         <is>
@@ -2105,10 +2105,10 @@
         <v>100</v>
       </c>
       <c r="Q22" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R22" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S22" s="0" t="inlineStr">
         <is>
@@ -4737,10 +4737,10 @@
         <v>100</v>
       </c>
       <c r="Q59" s="0">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R59" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S59" s="0" t="inlineStr">
         <is>
@@ -5163,10 +5163,10 @@
         <v>210</v>
       </c>
       <c r="Q65" s="0">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R65" s="0">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S65" s="0" t="inlineStr">
         <is>
@@ -5305,10 +5305,10 @@
         <v>500</v>
       </c>
       <c r="Q67" s="0">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="R67" s="0">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="S67" s="0" t="inlineStr">
         <is>
@@ -7151,10 +7151,10 @@
         <v>300</v>
       </c>
       <c r="Q93" s="0">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R93" s="0">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S93" s="0" t="inlineStr">
         <is>
@@ -10988,7 +10988,7 @@
         <v>23</v>
       </c>
       <c r="R147" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S147" s="0" t="inlineStr">
         <is>
@@ -12623,7 +12623,7 @@
         <v>100</v>
       </c>
       <c r="Q170" s="0">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R170" s="0">
         <v>93</v>
@@ -14966,10 +14966,10 @@
         <v>300</v>
       </c>
       <c r="Q203" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R203" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S203" s="0" t="inlineStr">
         <is>
@@ -15676,10 +15676,10 @@
         <v>2000</v>
       </c>
       <c r="Q213" s="0">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="R213" s="0">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="S213" s="0" t="inlineStr">
         <is>
@@ -17238,10 +17238,10 @@
         <v>200</v>
       </c>
       <c r="Q235" s="0">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R235" s="0">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S235" s="0" t="inlineStr">
         <is>
@@ -18161,10 +18161,10 @@
         <v>33</v>
       </c>
       <c r="Q248" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R248" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S248" s="0" t="inlineStr">
         <is>
@@ -24270,7 +24270,7 @@
         <v>9</v>
       </c>
       <c r="R334" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S334" s="0" t="inlineStr">
         <is>
@@ -25261,7 +25261,7 @@
         <v>10</v>
       </c>
       <c r="Q348" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R348" s="0">
         <v>4</v>
@@ -25685,7 +25685,7 @@
         <v>30</v>
       </c>
       <c r="R354" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S354" s="0" t="inlineStr">
         <is>

</xml_diff>